<commit_message>
Added web application files
</commit_message>
<xml_diff>
--- a/Database_mining/Example_Data/alaA_mutations.xlsx
+++ b/Database_mining/Example_Data/alaA_mutations.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitc-my.sharepoint.com/personal/kxmts01_cloud_uni-tuebingen_de/Documents/Dokumente/GitHub/CREATE_WebApplicaltion/Database_mining/Example_Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_1CF5E2F2F613C8264F2C4C2CAD40A75E79BCDD5D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19ED2435-4094-4385-9252-260A24EC7548}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -19,9 +25,6 @@
     <t>gene</t>
   </si>
   <si>
-    <t xml:space="preserve"> aa mutation</t>
-  </si>
-  <si>
     <t>position</t>
   </si>
   <si>
@@ -263,13 +266,16 @@
   </si>
   <si>
     <t>303</t>
+  </si>
+  <si>
+    <t>aa mutation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,17 +334,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -376,7 +390,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -410,6 +424,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -444,9 +459,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -619,582 +635,584 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>56</v>
       </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
         <v>18</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>57</v>
       </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="D16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>58</v>
       </c>
-      <c r="D16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
         <v>20</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
         <v>59</v>
       </c>
-      <c r="D17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>60</v>
-      </c>
-      <c r="D19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" t="s">
-        <v>61</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
         <v>28</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>66</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
         <v>29</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>67</v>
       </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
         <v>30</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>68</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
         <v>31</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>69</v>
       </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
         <v>32</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>70</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
         <v>33</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>71</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
         <v>34</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>72</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
         <v>35</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>73</v>
       </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
         <v>36</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>74</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
         <v>37</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>75</v>
       </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" t="s">
         <v>38</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>76</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
         <v>39</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>77</v>
       </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" t="s">
         <v>40</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>78</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
         <v>41</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>79</v>
       </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" t="s">
         <v>42</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>80</v>
       </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
         <v>43</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>81</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" t="s">
-        <v>44</v>
-      </c>
-      <c r="C41" t="s">
-        <v>82</v>
       </c>
       <c r="D41">
         <v>1</v>

</xml_diff>